<commit_message>
Added specific humidity to qc tests
</commit_message>
<xml_diff>
--- a/meta-data/flux-components-level1.xlsx
+++ b/meta-data/flux-components-level1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heather/Desktop/ARTofMELT/process-scripts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heather/Desktop/AOM-WP1-BL/meta-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEED903D-517E-8E4E-A4CB-16FCD1E720A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0628F570-8E6C-A246-879E-B99CE7B77301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1222" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1258" uniqueCount="193">
   <si>
     <t>Variable</t>
   </si>
@@ -553,18 +553,6 @@
     <t>bad_data good_data suspect_data</t>
   </si>
   <si>
-    <t>bad_data good_data  suspect_data</t>
-  </si>
-  <si>
-    <t>0, 1,  2</t>
-  </si>
-  <si>
-    <t>bad_data good_data good_for_reasearch suspect_data_good_for_general_use suspect_data_requires_further_checking_but_may_be_ok_for_general_use</t>
-  </si>
-  <si>
-    <t>0, 1, 2, 3</t>
-  </si>
-  <si>
     <t>thetaprime</t>
   </si>
   <si>
@@ -587,6 +575,30 @@
   </si>
   <si>
     <t>&lt;W'Theta'&gt;</t>
+  </si>
+  <si>
+    <t>qc_flag_skew_q</t>
+  </si>
+  <si>
+    <t>Quality flag: Skew Q</t>
+  </si>
+  <si>
+    <t>qc_flag_kurtosis_q</t>
+  </si>
+  <si>
+    <t>Quality flag: Kurtosis Q</t>
+  </si>
+  <si>
+    <t>0, 1,  2, 3</t>
+  </si>
+  <si>
+    <t>bad_data good_data _good_for_reasearch suspect_data_good_for_general_use suspect_data_requires_further_checking_but_may_be_ok_for_general_use</t>
+  </si>
+  <si>
+    <t>qc_flag_quality_wq</t>
+  </si>
+  <si>
+    <t>Quality flag: WQ</t>
   </si>
 </sst>
 </file>
@@ -645,7 +657,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -670,6 +682,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -688,9 +706,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -728,7 +746,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -834,7 +852,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -976,7 +994,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -989,8 +1007,8 @@
   </sheetPr>
   <dimension ref="A1:C965"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A618" workbookViewId="0">
-      <selection activeCell="C647" sqref="C647"/>
+    <sheetView tabSelected="1" topLeftCell="A745" workbookViewId="0">
+      <selection activeCell="O775" sqref="O775"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3606,7 +3624,7 @@
     <row r="366" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="367" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A367" s="8" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="368" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -3638,7 +3656,7 @@
         <v>11</v>
       </c>
       <c r="C371" s="8" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="372" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4152,7 +4170,7 @@
     <row r="443" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="444" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A444" s="8" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="445" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4184,7 +4202,7 @@
         <v>11</v>
       </c>
       <c r="C448" s="8" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="449" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4854,7 +4872,7 @@
     <row r="542" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="543" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A543" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="544" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4886,7 +4904,7 @@
         <v>11</v>
       </c>
       <c r="C547" s="8" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="548" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5556,7 +5574,7 @@
     <row r="641" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="642" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A642" s="8" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="643" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5588,7 +5606,7 @@
         <v>11</v>
       </c>
       <c r="C646" s="8" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="647" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5789,43 +5807,50 @@
     </row>
     <row r="674" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="675" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A675" t="s">
+      <c r="A675" s="2" t="s">
         <v>147</v>
       </c>
+      <c r="B675" s="2"/>
+      <c r="C675" s="10"/>
     </row>
     <row r="676" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B676" t="s">
-        <v>5</v>
-      </c>
-      <c r="C676" s="2" t="s">
+      <c r="A676" s="2"/>
+      <c r="B676" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C676" s="10" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="677" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B677" t="s">
-        <v>7</v>
-      </c>
-      <c r="C677" t="s">
+      <c r="A677" s="2"/>
+      <c r="B677" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C677" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="678" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B678" t="s">
-        <v>3</v>
-      </c>
-      <c r="C678" s="4">
+      <c r="A678" s="2"/>
+      <c r="B678" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C678" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="679" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B679" t="s">
-        <v>11</v>
-      </c>
-      <c r="C679" t="s">
+      <c r="A679" s="2"/>
+      <c r="B679" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C679" s="10" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="680" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A680" s="2"/>
       <c r="B680" s="2" t="s">
         <v>150</v>
       </c>
@@ -5842,45 +5867,54 @@
         <v>176</v>
       </c>
     </row>
-    <row r="682" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="682" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C682" s="10"/>
+    </row>
     <row r="683" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A683" t="s">
-        <v>152</v>
-      </c>
+      <c r="A683" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B683" s="2"/>
+      <c r="C683" s="10"/>
     </row>
     <row r="684" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B684" t="s">
-        <v>5</v>
-      </c>
-      <c r="C684" s="2" t="s">
+      <c r="A684" s="2"/>
+      <c r="B684" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C684" s="10" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="685" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B685" t="s">
-        <v>7</v>
-      </c>
-      <c r="C685" t="s">
+      <c r="A685" s="2"/>
+      <c r="B685" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C685" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="686" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B686" t="s">
-        <v>3</v>
-      </c>
-      <c r="C686" s="4">
+      <c r="A686" s="2"/>
+      <c r="B686" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C686" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="687" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B687" t="s">
-        <v>11</v>
-      </c>
-      <c r="C687" t="s">
-        <v>153</v>
+      <c r="A687" s="2"/>
+      <c r="B687" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C687" s="10" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="688" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A688" s="2"/>
       <c r="B688" s="2" t="s">
         <v>150</v>
       </c>
@@ -5889,52 +5923,64 @@
       </c>
     </row>
     <row r="689" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A689" s="2"/>
       <c r="B689" s="9" t="s">
         <v>151</v>
       </c>
       <c r="C689" s="6" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="690" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="690" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A690" s="2"/>
+      <c r="B690" s="2"/>
+      <c r="C690" s="10"/>
+    </row>
     <row r="691" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A691" t="s">
-        <v>154</v>
-      </c>
+      <c r="A691" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B691" s="2"/>
+      <c r="C691" s="10"/>
     </row>
     <row r="692" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B692" t="s">
-        <v>5</v>
-      </c>
-      <c r="C692" s="2" t="s">
+      <c r="A692" s="2"/>
+      <c r="B692" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C692" s="10" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="693" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B693" t="s">
-        <v>7</v>
-      </c>
-      <c r="C693" t="s">
+      <c r="A693" s="2"/>
+      <c r="B693" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C693" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="694" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B694" t="s">
-        <v>3</v>
-      </c>
-      <c r="C694" s="4">
+      <c r="A694" s="2"/>
+      <c r="B694" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C694" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="695" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B695" t="s">
-        <v>11</v>
-      </c>
-      <c r="C695" t="s">
-        <v>155</v>
+      <c r="A695" s="2"/>
+      <c r="B695" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C695" s="10" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="696" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A696" s="2"/>
       <c r="B696" s="2" t="s">
         <v>150</v>
       </c>
@@ -5943,60 +5989,73 @@
       </c>
     </row>
     <row r="697" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A697" s="2"/>
       <c r="B697" s="9" t="s">
         <v>151</v>
       </c>
       <c r="C697" s="6" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="698" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="698" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A698" s="2"/>
+      <c r="B698" s="2"/>
+      <c r="C698" s="10"/>
+    </row>
     <row r="699" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A699" t="s">
-        <v>156</v>
-      </c>
+      <c r="A699" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B699" s="2"/>
+      <c r="C699" s="10"/>
     </row>
     <row r="700" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B700" t="s">
-        <v>5</v>
-      </c>
-      <c r="C700" s="2" t="s">
+      <c r="A700" s="2"/>
+      <c r="B700" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C700" s="10" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="701" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B701" t="s">
-        <v>7</v>
-      </c>
-      <c r="C701" t="s">
+      <c r="A701" s="2"/>
+      <c r="B701" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C701" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="702" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B702" t="s">
-        <v>3</v>
-      </c>
-      <c r="C702" s="4">
+      <c r="A702" s="2"/>
+      <c r="B702" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C702" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="703" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B703" t="s">
-        <v>11</v>
-      </c>
-      <c r="C703" t="s">
-        <v>157</v>
+      <c r="A703" s="2"/>
+      <c r="B703" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C703" s="10" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="704" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A704" s="2"/>
       <c r="B704" s="2" t="s">
         <v>150</v>
       </c>
       <c r="C704" s="5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="705" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A705" s="2"/>
       <c r="B705" s="9" t="s">
         <v>151</v>
       </c>
@@ -6004,53 +6063,65 @@
         <v>176</v>
       </c>
     </row>
-    <row r="706" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="706" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A706" s="2"/>
+      <c r="B706" s="2"/>
+      <c r="C706" s="10"/>
+    </row>
     <row r="707" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A707" t="s">
-        <v>170</v>
-      </c>
+      <c r="A707" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B707" s="2"/>
+      <c r="C707" s="10"/>
     </row>
     <row r="708" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B708" t="s">
-        <v>5</v>
-      </c>
-      <c r="C708" s="2" t="s">
+      <c r="A708" s="2"/>
+      <c r="B708" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C708" s="10" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="709" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B709" t="s">
-        <v>7</v>
-      </c>
-      <c r="C709" t="s">
+      <c r="A709" s="2"/>
+      <c r="B709" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C709" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="710" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B710" t="s">
-        <v>3</v>
-      </c>
-      <c r="C710" s="4">
+      <c r="A710" s="2"/>
+      <c r="B710" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C710" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="711" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B711" t="s">
-        <v>11</v>
-      </c>
-      <c r="C711" t="s">
-        <v>158</v>
+      <c r="A711" s="2"/>
+      <c r="B711" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C711" s="10" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="712" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A712" s="2"/>
       <c r="B712" s="2" t="s">
         <v>150</v>
       </c>
       <c r="C712" s="5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="713" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A713" s="2"/>
       <c r="B713" s="9" t="s">
         <v>151</v>
       </c>
@@ -6058,53 +6129,65 @@
         <v>176</v>
       </c>
     </row>
-    <row r="714" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="714" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A714" s="2"/>
+      <c r="B714" s="2"/>
+      <c r="C714" s="10"/>
+    </row>
     <row r="715" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A715" t="s">
-        <v>171</v>
-      </c>
+      <c r="A715" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B715" s="2"/>
+      <c r="C715" s="10"/>
     </row>
     <row r="716" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B716" t="s">
-        <v>5</v>
-      </c>
-      <c r="C716" s="2" t="s">
+      <c r="A716" s="2"/>
+      <c r="B716" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C716" s="10" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="717" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B717" t="s">
-        <v>7</v>
-      </c>
-      <c r="C717" t="s">
+      <c r="A717" s="2"/>
+      <c r="B717" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C717" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="718" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B718" t="s">
-        <v>3</v>
-      </c>
-      <c r="C718" s="4">
+      <c r="A718" s="2"/>
+      <c r="B718" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C718" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="719" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B719" t="s">
-        <v>11</v>
-      </c>
-      <c r="C719" t="s">
-        <v>159</v>
+      <c r="A719" s="2"/>
+      <c r="B719" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C719" s="10" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="720" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A720" s="2"/>
       <c r="B720" s="2" t="s">
         <v>150</v>
       </c>
       <c r="C720" s="5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="721" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A721" s="2"/>
       <c r="B721" s="9" t="s">
         <v>151</v>
       </c>
@@ -6112,53 +6195,65 @@
         <v>176</v>
       </c>
     </row>
-    <row r="722" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="722" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A722" s="2"/>
+      <c r="B722" s="2"/>
+      <c r="C722" s="10"/>
+    </row>
     <row r="723" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A723" t="s">
-        <v>160</v>
-      </c>
+      <c r="A723" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B723" s="2"/>
+      <c r="C723" s="10"/>
     </row>
     <row r="724" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B724" t="s">
-        <v>5</v>
-      </c>
-      <c r="C724" s="2" t="s">
+      <c r="A724" s="2"/>
+      <c r="B724" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C724" s="10" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="725" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B725" t="s">
-        <v>7</v>
-      </c>
-      <c r="C725" t="s">
+      <c r="A725" s="2"/>
+      <c r="B725" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C725" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="726" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B726" t="s">
-        <v>3</v>
-      </c>
-      <c r="C726" s="4">
+      <c r="A726" s="2"/>
+      <c r="B726" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C726" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="727" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B727" t="s">
-        <v>11</v>
-      </c>
-      <c r="C727" t="s">
-        <v>161</v>
+      <c r="A727" s="2"/>
+      <c r="B727" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C727" s="10" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="728" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A728" s="2"/>
       <c r="B728" s="2" t="s">
         <v>150</v>
       </c>
       <c r="C728" s="5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="729" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A729" s="2"/>
       <c r="B729" s="9" t="s">
         <v>151</v>
       </c>
@@ -6166,45 +6261,56 @@
         <v>176</v>
       </c>
     </row>
-    <row r="730" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="730" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A730" s="2"/>
+      <c r="B730" s="2"/>
+      <c r="C730" s="10"/>
+    </row>
     <row r="731" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A731" t="s">
-        <v>162</v>
-      </c>
+      <c r="A731" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B731" s="2"/>
+      <c r="C731" s="10"/>
     </row>
     <row r="732" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B732" t="s">
-        <v>5</v>
-      </c>
-      <c r="C732" s="2" t="s">
+      <c r="A732" s="2"/>
+      <c r="B732" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C732" s="10" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="733" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B733" t="s">
-        <v>7</v>
-      </c>
-      <c r="C733" t="s">
+      <c r="A733" s="2"/>
+      <c r="B733" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C733" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="734" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B734" t="s">
-        <v>3</v>
-      </c>
-      <c r="C734" s="4">
+      <c r="A734" s="2"/>
+      <c r="B734" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C734" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="735" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B735" t="s">
-        <v>11</v>
-      </c>
-      <c r="C735" t="s">
-        <v>163</v>
+      <c r="A735" s="2"/>
+      <c r="B735" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C735" s="10" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="736" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A736" s="2"/>
       <c r="B736" s="2" t="s">
         <v>150</v>
       </c>
@@ -6213,6 +6319,7 @@
       </c>
     </row>
     <row r="737" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A737" s="2"/>
       <c r="B737" s="9" t="s">
         <v>151</v>
       </c>
@@ -6220,207 +6327,417 @@
         <v>176</v>
       </c>
     </row>
-    <row r="738" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="738" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A738" s="2"/>
+      <c r="B738" s="2"/>
+      <c r="C738" s="10"/>
+    </row>
     <row r="739" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A739" t="s">
-        <v>164</v>
-      </c>
+      <c r="A739" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B739" s="2"/>
+      <c r="C739" s="10"/>
     </row>
     <row r="740" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B740" t="s">
-        <v>5</v>
-      </c>
-      <c r="C740" s="2" t="s">
+      <c r="A740" s="2"/>
+      <c r="B740" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C740" s="10" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="741" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B741" t="s">
-        <v>7</v>
-      </c>
-      <c r="C741" t="s">
+      <c r="A741" s="2"/>
+      <c r="B741" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C741" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="742" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B742" t="s">
-        <v>3</v>
-      </c>
-      <c r="C742" s="4">
+      <c r="A742" s="2"/>
+      <c r="B742" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C742" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="743" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B743" t="s">
-        <v>11</v>
-      </c>
-      <c r="C743" t="s">
-        <v>165</v>
+      <c r="A743" s="2"/>
+      <c r="B743" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C743" s="10" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="744" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A744" s="2"/>
       <c r="B744" s="2" t="s">
         <v>150</v>
       </c>
       <c r="C744" s="5" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="745" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A745" s="2"/>
       <c r="B745" s="9" t="s">
         <v>151</v>
       </c>
       <c r="C745" s="6" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="746" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="746" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A746" s="2"/>
+      <c r="B746" s="2"/>
+      <c r="C746" s="10"/>
+    </row>
     <row r="747" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A747" t="s">
-        <v>166</v>
-      </c>
+      <c r="A747" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B747" s="2"/>
+      <c r="C747" s="10"/>
     </row>
     <row r="748" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B748" t="s">
-        <v>5</v>
-      </c>
-      <c r="C748" s="2" t="s">
+      <c r="A748" s="2"/>
+      <c r="B748" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C748" s="10" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="749" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B749" t="s">
-        <v>7</v>
-      </c>
-      <c r="C749" t="s">
+      <c r="A749" s="2"/>
+      <c r="B749" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C749" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="750" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B750" t="s">
-        <v>3</v>
-      </c>
-      <c r="C750" s="4">
+      <c r="A750" s="2"/>
+      <c r="B750" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C750" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="751" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B751" t="s">
-        <v>11</v>
-      </c>
-      <c r="C751" t="s">
-        <v>167</v>
+      <c r="A751" s="2"/>
+      <c r="B751" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C751" s="10" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="752" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A752" s="2"/>
       <c r="B752" s="2" t="s">
         <v>150</v>
       </c>
       <c r="C752" s="5" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="753" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A753" s="2"/>
       <c r="B753" s="9" t="s">
         <v>151</v>
       </c>
       <c r="C753" s="6" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="754" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="754" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A754" s="2"/>
+      <c r="B754" s="2"/>
+      <c r="C754" s="10"/>
+    </row>
     <row r="755" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A755" t="s">
-        <v>168</v>
-      </c>
+      <c r="A755" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B755" s="2"/>
+      <c r="C755" s="10"/>
     </row>
     <row r="756" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B756" t="s">
-        <v>5</v>
-      </c>
-      <c r="C756" s="2" t="s">
+      <c r="A756" s="2"/>
+      <c r="B756" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C756" s="10" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="757" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B757" t="s">
-        <v>7</v>
-      </c>
-      <c r="C757" t="s">
+      <c r="A757" s="2"/>
+      <c r="B757" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C757" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="758" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B758" t="s">
-        <v>3</v>
-      </c>
-      <c r="C758" s="4">
+      <c r="A758" s="2"/>
+      <c r="B758" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C758" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="759" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B759" t="s">
-        <v>11</v>
-      </c>
-      <c r="C759" t="s">
-        <v>169</v>
+      <c r="A759" s="2"/>
+      <c r="B759" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C759" s="10" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="760" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A760" s="2"/>
       <c r="B760" s="2" t="s">
         <v>150</v>
       </c>
       <c r="C760" s="5" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
     </row>
     <row r="761" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A761" s="2"/>
       <c r="B761" s="9" t="s">
         <v>151</v>
       </c>
       <c r="C761" s="6" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="762" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="763" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="764" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="765" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="766" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="767" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="768" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="769" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="770" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="771" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="772" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="773" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="774" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="775" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="776" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="777" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="778" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="779" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="780" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="781" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="782" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="783" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="784" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="785" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="786" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="787" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="788" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="789" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="790" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="791" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="792" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="793" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="794" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="795" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="796" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="797" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="798" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="799" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="800" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+        <v>190</v>
+      </c>
+    </row>
+    <row r="762" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A762" s="2"/>
+      <c r="B762" s="2"/>
+      <c r="C762" s="10"/>
+    </row>
+    <row r="763" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A763" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B763" s="2"/>
+      <c r="C763" s="10"/>
+    </row>
+    <row r="764" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A764" s="2"/>
+      <c r="B764" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C764" s="10" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="765" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A765" s="2"/>
+      <c r="B765" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C765" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="766" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A766" s="2"/>
+      <c r="B766" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C766" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="767" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A767" s="2"/>
+      <c r="B767" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C767" s="10" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="768" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A768" s="2"/>
+      <c r="B768" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C768" s="5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="769" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A769" s="2"/>
+      <c r="B769" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C769" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="770" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A770" s="2"/>
+      <c r="B770" s="2"/>
+      <c r="C770" s="10"/>
+    </row>
+    <row r="771" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A771" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B771" s="2"/>
+      <c r="C771" s="10"/>
+    </row>
+    <row r="772" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A772" s="2"/>
+      <c r="B772" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C772" s="10" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="773" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A773" s="2"/>
+      <c r="B773" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C773" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="774" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A774" s="2"/>
+      <c r="B774" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C774" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="775" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A775" s="2"/>
+      <c r="B775" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C775" s="10" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="776" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A776" s="2"/>
+      <c r="B776" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C776" s="5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="777" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A777" s="2"/>
+      <c r="B777" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C777" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="778" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A778" s="2"/>
+      <c r="B778" s="2"/>
+      <c r="C778" s="10"/>
+    </row>
+    <row r="779" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A779" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B779" s="2"/>
+      <c r="C779" s="10"/>
+    </row>
+    <row r="780" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A780" s="2"/>
+      <c r="B780" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C780" s="10" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="781" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A781" s="2"/>
+      <c r="B781" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C781" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="782" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A782" s="2"/>
+      <c r="B782" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C782" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="783" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A783" s="2"/>
+      <c r="B783" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C783" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="784" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A784" s="2"/>
+      <c r="B784" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C784" s="5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="785" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A785" s="2"/>
+      <c r="B785" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C785" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="786" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="787" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="788" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="789" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="790" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="791" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="792" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="793" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="794" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="795" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="796" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="797" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="798" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="799" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="800" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="801" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="802" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="803" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
add specific humidity stats
</commit_message>
<xml_diff>
--- a/meta-data/flux-components-level1.xlsx
+++ b/meta-data/flux-components-level1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heather/Desktop/AOM-WP1-BL/meta-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0628F570-8E6C-A246-879E-B99CE7B77301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{128D6DC4-2E3D-6543-8B91-4968A790510C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="32780" windowHeight="18860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="variables-specific" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1258" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1309" uniqueCount="199">
   <si>
     <t>Variable</t>
   </si>
@@ -599,6 +599,24 @@
   </si>
   <si>
     <t>Quality flag: WQ</t>
+  </si>
+  <si>
+    <t>sst_wq</t>
+  </si>
+  <si>
+    <t>Steady State Test Result Wq</t>
+  </si>
+  <si>
+    <t>kurtosis_specific_humidity</t>
+  </si>
+  <si>
+    <t>Kurtosis Specific Humidity (Q)</t>
+  </si>
+  <si>
+    <t>skew_specific_humidity</t>
+  </si>
+  <si>
+    <t>Skew Specific Humidity (Q)</t>
   </si>
 </sst>
 </file>
@@ -1007,8 +1025,8 @@
   </sheetPr>
   <dimension ref="A1:C965"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A745" workbookViewId="0">
-      <selection activeCell="O775" sqref="O775"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="C196" sqref="C196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2376,7 +2394,7 @@
     <row r="190" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="191" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A191" s="2" t="s">
-        <v>60</v>
+        <v>197</v>
       </c>
     </row>
     <row r="192" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -2408,7 +2426,7 @@
         <v>11</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>61</v>
+        <v>198</v>
       </c>
     </row>
     <row r="196" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -2454,7 +2472,7 @@
     <row r="201" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="202" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A202" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="203" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -2486,7 +2504,7 @@
         <v>11</v>
       </c>
       <c r="C206" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="207" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -2532,7 +2550,7 @@
     <row r="212" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="213" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A213" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="214" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -2564,7 +2582,7 @@
         <v>11</v>
       </c>
       <c r="C217" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="218" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -2610,7 +2628,7 @@
     <row r="223" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="224" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A224" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="225" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -2642,7 +2660,7 @@
         <v>11</v>
       </c>
       <c r="C228" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="229" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -2687,8 +2705,8 @@
     </row>
     <row r="234" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="235" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A235" t="s">
-        <v>68</v>
+      <c r="A235" s="2" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="236" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -2719,8 +2737,8 @@
       <c r="B239" t="s">
         <v>11</v>
       </c>
-      <c r="C239" t="s">
-        <v>69</v>
+      <c r="C239" s="2" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="240" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -2765,8 +2783,8 @@
     </row>
     <row r="245" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="246" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A246" t="s">
-        <v>70</v>
+      <c r="A246" s="2" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="247" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -2797,8 +2815,8 @@
       <c r="B250" t="s">
         <v>11</v>
       </c>
-      <c r="C250" t="s">
-        <v>71</v>
+      <c r="C250" s="2" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="251" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -2844,7 +2862,7 @@
     <row r="256" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="257" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A257" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="258" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -2876,7 +2894,7 @@
         <v>11</v>
       </c>
       <c r="C261" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="262" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -2922,7 +2940,7 @@
     <row r="267" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="268" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A268" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="269" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -2945,16 +2963,16 @@
       <c r="B271" t="s">
         <v>3</v>
       </c>
-      <c r="C271" s="4" t="s">
-        <v>45</v>
+      <c r="C271" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="272" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B272" t="s">
         <v>11</v>
       </c>
-      <c r="C272" s="2" t="s">
-        <v>75</v>
+      <c r="C272" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="273" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -3000,7 +3018,7 @@
     <row r="278" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="279" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A279" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="280" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -3023,16 +3041,16 @@
       <c r="B282" t="s">
         <v>3</v>
       </c>
-      <c r="C282" s="4" t="s">
-        <v>77</v>
+      <c r="C282" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="283" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B283" t="s">
         <v>11</v>
       </c>
-      <c r="C283" s="2" t="s">
-        <v>78</v>
+      <c r="C283" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="284" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -3077,8 +3095,8 @@
     </row>
     <row r="289" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="290" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A290" t="s">
-        <v>79</v>
+      <c r="A290" s="8" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="291" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -3109,8 +3127,8 @@
       <c r="B294" t="s">
         <v>11</v>
       </c>
-      <c r="C294" s="2" t="s">
-        <v>80</v>
+      <c r="C294" s="8" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="295" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -3155,8 +3173,8 @@
     </row>
     <row r="300" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="301" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A301" s="2" t="s">
-        <v>81</v>
+      <c r="A301" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="302" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -3188,7 +3206,7 @@
         <v>11</v>
       </c>
       <c r="C305" s="2" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="306" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -3220,7 +3238,7 @@
         <v>26</v>
       </c>
       <c r="C309" t="s">
-        <v>83</v>
+        <v>27</v>
       </c>
     </row>
     <row r="310" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -3233,8 +3251,8 @@
     </row>
     <row r="311" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="312" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A312" s="2" t="s">
-        <v>84</v>
+      <c r="A312" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="313" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -3257,8 +3275,8 @@
       <c r="B315" t="s">
         <v>3</v>
       </c>
-      <c r="C315" s="4">
-        <v>1</v>
+      <c r="C315" s="4" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="316" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -3266,7 +3284,7 @@
         <v>11</v>
       </c>
       <c r="C316" s="2" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="317" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -3312,7 +3330,7 @@
     <row r="322" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="323" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A323" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="324" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -3335,16 +3353,16 @@
       <c r="B326" t="s">
         <v>3</v>
       </c>
-      <c r="C326" s="4" t="s">
-        <v>45</v>
+      <c r="C326" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="327" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B327" t="s">
         <v>11</v>
       </c>
-      <c r="C327" t="s">
-        <v>87</v>
+      <c r="C327" s="2" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="328" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -3376,7 +3394,7 @@
         <v>26</v>
       </c>
       <c r="C331" t="s">
-        <v>88</v>
+        <v>27</v>
       </c>
     </row>
     <row r="332" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -3389,8 +3407,8 @@
     </row>
     <row r="333" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="334" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A334" t="s">
-        <v>89</v>
+      <c r="A334" s="2" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="335" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -3421,8 +3439,8 @@
       <c r="B338" t="s">
         <v>11</v>
       </c>
-      <c r="C338" t="s">
-        <v>90</v>
+      <c r="C338" s="2" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="339" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -3454,7 +3472,7 @@
         <v>26</v>
       </c>
       <c r="C342" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="343" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -3467,8 +3485,8 @@
     </row>
     <row r="344" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="345" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A345" t="s">
-        <v>91</v>
+      <c r="A345" s="2" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="346" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -3491,16 +3509,16 @@
       <c r="B348" t="s">
         <v>3</v>
       </c>
-      <c r="C348" s="4" t="s">
-        <v>45</v>
+      <c r="C348" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="349" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B349" t="s">
         <v>11</v>
       </c>
-      <c r="C349" t="s">
-        <v>92</v>
+      <c r="C349" s="2" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="350" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -3532,7 +3550,7 @@
         <v>26</v>
       </c>
       <c r="C353" t="s">
-        <v>88</v>
+        <v>27</v>
       </c>
     </row>
     <row r="354" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -3546,7 +3564,7 @@
     <row r="355" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="356" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A356" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="357" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -3570,7 +3588,7 @@
         <v>3</v>
       </c>
       <c r="C359" s="4" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
     </row>
     <row r="360" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -3578,7 +3596,7 @@
         <v>11</v>
       </c>
       <c r="C360" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="361" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -3623,8 +3641,8 @@
     </row>
     <row r="366" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="367" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A367" s="8" t="s">
-        <v>181</v>
+      <c r="A367" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="368" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -3648,15 +3666,15 @@
         <v>3</v>
       </c>
       <c r="C370" s="4" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
     </row>
     <row r="371" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B371" t="s">
         <v>11</v>
       </c>
-      <c r="C371" s="8" t="s">
-        <v>182</v>
+      <c r="C371" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="372" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -3702,7 +3720,7 @@
     <row r="377" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="378" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A378" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="379" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -3726,7 +3744,7 @@
         <v>3</v>
       </c>
       <c r="C381" s="4" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
     </row>
     <row r="382" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -3734,7 +3752,7 @@
         <v>11</v>
       </c>
       <c r="C382" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="383" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -3779,8 +3797,8 @@
     </row>
     <row r="388" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="389" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A389" s="2" t="s">
-        <v>97</v>
+      <c r="A389" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="390" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -3804,7 +3822,7 @@
         <v>3</v>
       </c>
       <c r="C392" s="4" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="393" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -3812,7 +3830,7 @@
         <v>11</v>
       </c>
       <c r="C393" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="394" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -3857,8 +3875,8 @@
     </row>
     <row r="399" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="400" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A400" t="s">
-        <v>99</v>
+      <c r="A400" s="8" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="401" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -3874,7 +3892,7 @@
         <v>7</v>
       </c>
       <c r="C402" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
     </row>
     <row r="403" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -3882,15 +3900,15 @@
         <v>3</v>
       </c>
       <c r="C403" s="4" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
     </row>
     <row r="404" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B404" t="s">
         <v>11</v>
       </c>
-      <c r="C404" t="s">
-        <v>100</v>
+      <c r="C404" s="8" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="405" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -3922,7 +3940,7 @@
         <v>26</v>
       </c>
       <c r="C408" t="s">
-        <v>27</v>
+        <v>88</v>
       </c>
     </row>
     <row r="409" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -3936,7 +3954,7 @@
     <row r="410" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="411" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A411" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="412" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -3952,7 +3970,7 @@
         <v>7</v>
       </c>
       <c r="C413" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
     </row>
     <row r="414" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -3960,7 +3978,7 @@
         <v>3</v>
       </c>
       <c r="C414" s="4" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
     </row>
     <row r="415" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -3968,7 +3986,7 @@
         <v>11</v>
       </c>
       <c r="C415" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="416" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4000,7 +4018,7 @@
         <v>26</v>
       </c>
       <c r="C419" t="s">
-        <v>27</v>
+        <v>88</v>
       </c>
     </row>
     <row r="420" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4013,8 +4031,8 @@
     </row>
     <row r="421" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="422" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A422" t="s">
-        <v>103</v>
+      <c r="A422" s="2" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="423" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4030,7 +4048,7 @@
         <v>7</v>
       </c>
       <c r="C424" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
     </row>
     <row r="425" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4038,7 +4056,7 @@
         <v>3</v>
       </c>
       <c r="C425" s="4" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="426" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4046,7 +4064,7 @@
         <v>11</v>
       </c>
       <c r="C426" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="427" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4078,7 +4096,7 @@
         <v>26</v>
       </c>
       <c r="C430" t="s">
-        <v>27</v>
+        <v>88</v>
       </c>
     </row>
     <row r="431" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4092,7 +4110,7 @@
     <row r="432" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="433" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A433" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="434" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4116,7 +4134,7 @@
         <v>3</v>
       </c>
       <c r="C436" s="4" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
     </row>
     <row r="437" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4124,7 +4142,7 @@
         <v>11</v>
       </c>
       <c r="C437" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="438" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4169,8 +4187,8 @@
     </row>
     <row r="443" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="444" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A444" s="8" t="s">
-        <v>177</v>
+      <c r="A444" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="445" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4194,15 +4212,15 @@
         <v>3</v>
       </c>
       <c r="C447" s="4" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
     </row>
     <row r="448" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B448" t="s">
         <v>11</v>
       </c>
-      <c r="C448" s="8" t="s">
-        <v>178</v>
+      <c r="C448" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="449" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4248,7 +4266,7 @@
     <row r="454" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="455" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A455" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="456" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4272,7 +4290,7 @@
         <v>3</v>
       </c>
       <c r="C458" s="4" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
     </row>
     <row r="459" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4280,7 +4298,7 @@
         <v>11</v>
       </c>
       <c r="C459" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="460" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4325,8 +4343,8 @@
     </row>
     <row r="465" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="466" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A466" s="2" t="s">
-        <v>109</v>
+      <c r="A466" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="467" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4350,7 +4368,7 @@
         <v>3</v>
       </c>
       <c r="C469" s="4" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="470" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4358,7 +4376,7 @@
         <v>11</v>
       </c>
       <c r="C470" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="471" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4403,8 +4421,8 @@
     </row>
     <row r="476" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="477" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A477" t="s">
-        <v>111</v>
+      <c r="A477" s="8" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="478" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4428,15 +4446,15 @@
         <v>3</v>
       </c>
       <c r="C480" s="4" t="s">
-        <v>112</v>
+        <v>25</v>
       </c>
     </row>
     <row r="481" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B481" t="s">
         <v>11</v>
       </c>
-      <c r="C481" t="s">
-        <v>113</v>
+      <c r="C481" s="8" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="482" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4482,7 +4500,7 @@
     <row r="487" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="488" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A488" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="489" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4506,7 +4524,7 @@
         <v>3</v>
       </c>
       <c r="C491" s="4" t="s">
-        <v>112</v>
+        <v>31</v>
       </c>
     </row>
     <row r="492" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4514,7 +4532,7 @@
         <v>11</v>
       </c>
       <c r="C492" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="493" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4559,8 +4577,8 @@
     </row>
     <row r="498" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="499" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A499" t="s">
-        <v>116</v>
+      <c r="A499" s="2" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="500" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4584,7 +4602,7 @@
         <v>3</v>
       </c>
       <c r="C502" s="4" t="s">
-        <v>112</v>
+        <v>35</v>
       </c>
     </row>
     <row r="503" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4592,7 +4610,7 @@
         <v>11</v>
       </c>
       <c r="C503" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="504" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4638,7 +4656,7 @@
     <row r="509" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="510" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A510" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="511" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4670,7 +4688,7 @@
         <v>11</v>
       </c>
       <c r="C514" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="515" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4716,7 +4734,7 @@
     <row r="520" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="521" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A521" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="522" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4748,7 +4766,7 @@
         <v>11</v>
       </c>
       <c r="C525" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="526" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4794,7 +4812,7 @@
     <row r="531" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="532" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A532" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="533" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4818,7 +4836,7 @@
         <v>3</v>
       </c>
       <c r="C535" s="4" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
     </row>
     <row r="536" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4826,7 +4844,7 @@
         <v>11</v>
       </c>
       <c r="C536" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="537" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4872,7 +4890,7 @@
     <row r="542" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="543" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A543" t="s">
-        <v>179</v>
+        <v>118</v>
       </c>
     </row>
     <row r="544" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4896,15 +4914,15 @@
         <v>3</v>
       </c>
       <c r="C546" s="4" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
     </row>
     <row r="547" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B547" t="s">
         <v>11</v>
       </c>
-      <c r="C547" s="8" t="s">
-        <v>180</v>
+      <c r="C547" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="548" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4950,7 +4968,7 @@
     <row r="553" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="554" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A554" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="555" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4974,7 +4992,7 @@
         <v>3</v>
       </c>
       <c r="C557" s="4" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
     </row>
     <row r="558" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4982,7 +5000,7 @@
         <v>11</v>
       </c>
       <c r="C558" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="559" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5027,8 +5045,8 @@
     </row>
     <row r="564" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="565" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A565" s="2" t="s">
-        <v>128</v>
+      <c r="A565" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="566" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5052,7 +5070,7 @@
         <v>3</v>
       </c>
       <c r="C568" s="4" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="569" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5060,7 +5078,7 @@
         <v>11</v>
       </c>
       <c r="C569" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="570" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5106,7 +5124,7 @@
     <row r="575" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="576" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A576" t="s">
-        <v>131</v>
+        <v>179</v>
       </c>
     </row>
     <row r="577" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5122,7 +5140,7 @@
         <v>7</v>
       </c>
       <c r="C578" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
     </row>
     <row r="579" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5130,15 +5148,15 @@
         <v>3</v>
       </c>
       <c r="C579" s="4" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
     </row>
     <row r="580" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B580" t="s">
         <v>11</v>
       </c>
-      <c r="C580" t="s">
-        <v>132</v>
+      <c r="C580" s="8" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="581" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5170,7 +5188,7 @@
         <v>26</v>
       </c>
       <c r="C584" t="s">
-        <v>88</v>
+        <v>27</v>
       </c>
     </row>
     <row r="585" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5184,7 +5202,7 @@
     <row r="586" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="587" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A587" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
     </row>
     <row r="588" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5200,7 +5218,7 @@
         <v>7</v>
       </c>
       <c r="C589" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
     </row>
     <row r="590" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5208,7 +5226,7 @@
         <v>3</v>
       </c>
       <c r="C590" s="4" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
     </row>
     <row r="591" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5216,7 +5234,7 @@
         <v>11</v>
       </c>
       <c r="C591" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="592" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5248,7 +5266,7 @@
         <v>26</v>
       </c>
       <c r="C595" t="s">
-        <v>88</v>
+        <v>27</v>
       </c>
     </row>
     <row r="596" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5261,8 +5279,8 @@
     </row>
     <row r="597" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="598" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A598" t="s">
-        <v>135</v>
+      <c r="A598" s="2" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="599" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5278,7 +5296,7 @@
         <v>7</v>
       </c>
       <c r="C600" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
     </row>
     <row r="601" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5286,7 +5304,7 @@
         <v>3</v>
       </c>
       <c r="C601" s="4" t="s">
-        <v>112</v>
+        <v>129</v>
       </c>
     </row>
     <row r="602" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5294,7 +5312,7 @@
         <v>11</v>
       </c>
       <c r="C602" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="603" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5326,7 +5344,7 @@
         <v>26</v>
       </c>
       <c r="C606" t="s">
-        <v>88</v>
+        <v>27</v>
       </c>
     </row>
     <row r="607" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5340,7 +5358,7 @@
     <row r="608" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="609" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A609" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="610" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5372,7 +5390,7 @@
         <v>11</v>
       </c>
       <c r="C613" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="614" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5418,7 +5436,7 @@
     <row r="619" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="620" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A620" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="621" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5450,7 +5468,7 @@
         <v>11</v>
       </c>
       <c r="C624" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="625" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5496,7 +5514,7 @@
     <row r="630" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="631" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A631" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="632" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5520,7 +5538,7 @@
         <v>3</v>
       </c>
       <c r="C634" s="4" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
     </row>
     <row r="635" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5528,7 +5546,7 @@
         <v>11</v>
       </c>
       <c r="C635" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="636" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5573,8 +5591,8 @@
     </row>
     <row r="641" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="642" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A642" s="8" t="s">
-        <v>183</v>
+      <c r="A642" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="643" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5598,15 +5616,15 @@
         <v>3</v>
       </c>
       <c r="C645" s="4" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
     </row>
     <row r="646" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B646" t="s">
         <v>11</v>
       </c>
-      <c r="C646" s="8" t="s">
-        <v>184</v>
+      <c r="C646" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="647" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5652,7 +5670,7 @@
     <row r="652" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="653" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A653" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="654" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5676,7 +5694,7 @@
         <v>3</v>
       </c>
       <c r="C656" s="4" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
     </row>
     <row r="657" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5684,7 +5702,7 @@
         <v>11</v>
       </c>
       <c r="C657" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="658" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5729,8 +5747,8 @@
     </row>
     <row r="663" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="664" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A664" s="2" t="s">
-        <v>145</v>
+      <c r="A664" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="665" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5754,7 +5772,7 @@
         <v>3</v>
       </c>
       <c r="C667" s="4" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="668" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5762,7 +5780,7 @@
         <v>11</v>
       </c>
       <c r="C668" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="669" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5807,969 +5825,1170 @@
     </row>
     <row r="674" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="675" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A675" s="2" t="s">
+      <c r="A675" s="8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="676" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B676" t="s">
+        <v>5</v>
+      </c>
+      <c r="C676" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="677" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B677" t="s">
+        <v>7</v>
+      </c>
+      <c r="C677" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="678" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B678" t="s">
+        <v>3</v>
+      </c>
+      <c r="C678" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="679" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B679" t="s">
+        <v>11</v>
+      </c>
+      <c r="C679" s="8" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="680" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B680" t="s">
+        <v>13</v>
+      </c>
+      <c r="C680" s="3">
+        <v>-1E+20</v>
+      </c>
+    </row>
+    <row r="681" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B681" t="s">
+        <v>14</v>
+      </c>
+      <c r="C681" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="682" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B682" t="s">
+        <v>15</v>
+      </c>
+      <c r="C682" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="683" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B683" t="s">
+        <v>26</v>
+      </c>
+      <c r="C683" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="684" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B684" t="s">
+        <v>16</v>
+      </c>
+      <c r="C684" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="685" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="686" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A686" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="687" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B687" t="s">
+        <v>5</v>
+      </c>
+      <c r="C687" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="688" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B688" t="s">
+        <v>7</v>
+      </c>
+      <c r="C688" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="689" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B689" t="s">
+        <v>3</v>
+      </c>
+      <c r="C689" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="690" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B690" t="s">
+        <v>11</v>
+      </c>
+      <c r="C690" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="691" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B691" t="s">
+        <v>13</v>
+      </c>
+      <c r="C691" s="3">
+        <v>-1E+20</v>
+      </c>
+    </row>
+    <row r="692" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B692" t="s">
+        <v>14</v>
+      </c>
+      <c r="C692" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="693" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B693" t="s">
+        <v>15</v>
+      </c>
+      <c r="C693" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="694" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B694" t="s">
+        <v>26</v>
+      </c>
+      <c r="C694" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="695" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B695" t="s">
+        <v>16</v>
+      </c>
+      <c r="C695" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="696" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="697" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A697" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="698" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B698" t="s">
+        <v>5</v>
+      </c>
+      <c r="C698" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="699" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B699" t="s">
+        <v>7</v>
+      </c>
+      <c r="C699" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="700" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B700" t="s">
+        <v>3</v>
+      </c>
+      <c r="C700" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="701" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B701" t="s">
+        <v>11</v>
+      </c>
+      <c r="C701" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="702" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B702" t="s">
+        <v>13</v>
+      </c>
+      <c r="C702" s="3">
+        <v>-1E+20</v>
+      </c>
+    </row>
+    <row r="703" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B703" t="s">
+        <v>14</v>
+      </c>
+      <c r="C703" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="704" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B704" t="s">
+        <v>15</v>
+      </c>
+      <c r="C704" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="705" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B705" t="s">
+        <v>26</v>
+      </c>
+      <c r="C705" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="706" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B706" t="s">
+        <v>16</v>
+      </c>
+      <c r="C706" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="707" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="708" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A708" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B675" s="2"/>
-      <c r="C675" s="10"/>
-    </row>
-    <row r="676" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A676" s="2"/>
-      <c r="B676" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C676" s="10" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="677" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A677" s="2"/>
-      <c r="B677" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C677" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="678" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A678" s="2"/>
-      <c r="B678" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C678" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="679" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A679" s="2"/>
-      <c r="B679" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C679" s="10" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="680" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A680" s="2"/>
-      <c r="B680" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="C680" s="5" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="681" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A681" s="2"/>
-      <c r="B681" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="C681" s="6" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="682" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C682" s="10"/>
-    </row>
-    <row r="683" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A683" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="B683" s="2"/>
-      <c r="C683" s="10"/>
-    </row>
-    <row r="684" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A684" s="2"/>
-      <c r="B684" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C684" s="10" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="685" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A685" s="2"/>
-      <c r="B685" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C685" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="686" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A686" s="2"/>
-      <c r="B686" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C686" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="687" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A687" s="2"/>
-      <c r="B687" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C687" s="10" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="688" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A688" s="2"/>
-      <c r="B688" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="C688" s="5" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="689" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A689" s="2"/>
-      <c r="B689" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="C689" s="6" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="690" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A690" s="2"/>
-      <c r="B690" s="2"/>
-      <c r="C690" s="10"/>
-    </row>
-    <row r="691" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A691" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="B691" s="2"/>
-      <c r="C691" s="10"/>
-    </row>
-    <row r="692" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A692" s="2"/>
-      <c r="B692" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C692" s="10" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="693" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A693" s="2"/>
-      <c r="B693" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C693" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="694" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A694" s="2"/>
-      <c r="B694" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C694" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="695" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A695" s="2"/>
-      <c r="B695" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C695" s="10" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="696" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A696" s="2"/>
-      <c r="B696" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="C696" s="5" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="697" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A697" s="2"/>
-      <c r="B697" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="C697" s="6" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="698" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A698" s="2"/>
-      <c r="B698" s="2"/>
-      <c r="C698" s="10"/>
-    </row>
-    <row r="699" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A699" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="B699" s="2"/>
-      <c r="C699" s="10"/>
-    </row>
-    <row r="700" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A700" s="2"/>
-      <c r="B700" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C700" s="10" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="701" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A701" s="2"/>
-      <c r="B701" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C701" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="702" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A702" s="2"/>
-      <c r="B702" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C702" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="703" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A703" s="2"/>
-      <c r="B703" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C703" s="10" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="704" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A704" s="2"/>
-      <c r="B704" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="C704" s="5" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="705" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A705" s="2"/>
-      <c r="B705" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="C705" s="6" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="706" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A706" s="2"/>
-      <c r="B706" s="2"/>
-      <c r="C706" s="10"/>
-    </row>
-    <row r="707" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A707" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B707" s="2"/>
-      <c r="C707" s="10"/>
-    </row>
-    <row r="708" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A708" s="2"/>
-      <c r="B708" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C708" s="10" t="s">
-        <v>148</v>
-      </c>
+      <c r="B708" s="2"/>
+      <c r="C708" s="10"/>
     </row>
     <row r="709" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A709" s="2"/>
       <c r="B709" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C709" s="10" t="s">
-        <v>8</v>
+        <v>148</v>
       </c>
     </row>
     <row r="710" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A710" s="2"/>
       <c r="B710" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C710" s="11">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="C710" s="10" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="711" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A711" s="2"/>
       <c r="B711" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C711" s="10" t="s">
-        <v>157</v>
+        <v>3</v>
+      </c>
+      <c r="C711" s="11">
+        <v>1</v>
       </c>
     </row>
     <row r="712" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A712" s="2"/>
       <c r="B712" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="C712" s="5" t="s">
-        <v>175</v>
+        <v>11</v>
+      </c>
+      <c r="C712" s="10" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="713" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A713" s="2"/>
-      <c r="B713" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="C713" s="6" t="s">
-        <v>176</v>
+      <c r="B713" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C713" s="5" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="714" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A714" s="2"/>
-      <c r="B714" s="2"/>
-      <c r="C714" s="10"/>
+      <c r="B714" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C714" s="6" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="715" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A715" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="B715" s="2"/>
       <c r="C715" s="10"/>
     </row>
     <row r="716" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A716" s="2"/>
-      <c r="B716" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C716" s="10" t="s">
-        <v>148</v>
-      </c>
+      <c r="A716" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B716" s="2"/>
+      <c r="C716" s="10"/>
     </row>
     <row r="717" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A717" s="2"/>
       <c r="B717" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C717" s="10" t="s">
-        <v>8</v>
+        <v>148</v>
       </c>
     </row>
     <row r="718" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A718" s="2"/>
       <c r="B718" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C718" s="11">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="C718" s="10" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="719" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A719" s="2"/>
       <c r="B719" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C719" s="10" t="s">
-        <v>158</v>
+        <v>3</v>
+      </c>
+      <c r="C719" s="11">
+        <v>1</v>
       </c>
     </row>
     <row r="720" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A720" s="2"/>
       <c r="B720" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="C720" s="5" t="s">
-        <v>175</v>
+        <v>11</v>
+      </c>
+      <c r="C720" s="10" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="721" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A721" s="2"/>
-      <c r="B721" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="C721" s="6" t="s">
-        <v>176</v>
+      <c r="B721" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C721" s="5" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="722" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A722" s="2"/>
-      <c r="B722" s="2"/>
-      <c r="C722" s="10"/>
+      <c r="B722" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C722" s="6" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="723" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A723" s="2" t="s">
-        <v>187</v>
-      </c>
+      <c r="A723" s="2"/>
       <c r="B723" s="2"/>
       <c r="C723" s="10"/>
     </row>
     <row r="724" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A724" s="2"/>
-      <c r="B724" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C724" s="10" t="s">
-        <v>148</v>
-      </c>
+      <c r="A724" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B724" s="2"/>
+      <c r="C724" s="10"/>
     </row>
     <row r="725" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A725" s="2"/>
       <c r="B725" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C725" s="10" t="s">
-        <v>8</v>
+        <v>148</v>
       </c>
     </row>
     <row r="726" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A726" s="2"/>
       <c r="B726" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C726" s="11">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="C726" s="10" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="727" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A727" s="2"/>
       <c r="B727" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C727" s="10" t="s">
-        <v>188</v>
+        <v>3</v>
+      </c>
+      <c r="C727" s="11">
+        <v>1</v>
       </c>
     </row>
     <row r="728" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A728" s="2"/>
       <c r="B728" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="C728" s="5" t="s">
-        <v>175</v>
+        <v>11</v>
+      </c>
+      <c r="C728" s="10" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="729" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A729" s="2"/>
-      <c r="B729" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="C729" s="6" t="s">
-        <v>176</v>
+      <c r="B729" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C729" s="5" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="730" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A730" s="2"/>
-      <c r="B730" s="2"/>
-      <c r="C730" s="10"/>
+      <c r="B730" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C730" s="6" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="731" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A731" s="2" t="s">
-        <v>171</v>
-      </c>
+      <c r="A731" s="2"/>
       <c r="B731" s="2"/>
       <c r="C731" s="10"/>
     </row>
     <row r="732" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A732" s="2"/>
-      <c r="B732" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C732" s="10" t="s">
-        <v>148</v>
-      </c>
+      <c r="A732" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B732" s="2"/>
+      <c r="C732" s="10"/>
     </row>
     <row r="733" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A733" s="2"/>
       <c r="B733" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C733" s="10" t="s">
-        <v>8</v>
+        <v>148</v>
       </c>
     </row>
     <row r="734" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A734" s="2"/>
       <c r="B734" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C734" s="11">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="C734" s="10" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="735" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A735" s="2"/>
       <c r="B735" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C735" s="10" t="s">
-        <v>159</v>
+        <v>3</v>
+      </c>
+      <c r="C735" s="11">
+        <v>1</v>
       </c>
     </row>
     <row r="736" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A736" s="2"/>
       <c r="B736" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="C736" s="5" t="s">
-        <v>175</v>
+        <v>11</v>
+      </c>
+      <c r="C736" s="10" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="737" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A737" s="2"/>
-      <c r="B737" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="C737" s="6" t="s">
-        <v>176</v>
+      <c r="B737" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C737" s="5" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="738" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A738" s="2"/>
-      <c r="B738" s="2"/>
-      <c r="C738" s="10"/>
+      <c r="B738" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C738" s="6" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="739" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A739" s="2" t="s">
-        <v>160</v>
-      </c>
+      <c r="A739" s="2"/>
       <c r="B739" s="2"/>
       <c r="C739" s="10"/>
     </row>
     <row r="740" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A740" s="2"/>
-      <c r="B740" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C740" s="10" t="s">
-        <v>148</v>
-      </c>
+      <c r="A740" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B740" s="2"/>
+      <c r="C740" s="10"/>
     </row>
     <row r="741" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A741" s="2"/>
       <c r="B741" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C741" s="10" t="s">
-        <v>8</v>
+        <v>148</v>
       </c>
     </row>
     <row r="742" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A742" s="2"/>
       <c r="B742" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C742" s="11">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="C742" s="10" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="743" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A743" s="2"/>
       <c r="B743" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C743" s="10" t="s">
-        <v>161</v>
+        <v>3</v>
+      </c>
+      <c r="C743" s="11">
+        <v>1</v>
       </c>
     </row>
     <row r="744" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A744" s="2"/>
       <c r="B744" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="C744" s="5" t="s">
-        <v>175</v>
+        <v>11</v>
+      </c>
+      <c r="C744" s="10" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="745" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A745" s="2"/>
-      <c r="B745" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="C745" s="6" t="s">
-        <v>176</v>
+      <c r="B745" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C745" s="5" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="746" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A746" s="2"/>
-      <c r="B746" s="2"/>
-      <c r="C746" s="10"/>
+      <c r="B746" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C746" s="6" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="747" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A747" s="2" t="s">
-        <v>162</v>
-      </c>
+      <c r="A747" s="2"/>
       <c r="B747" s="2"/>
       <c r="C747" s="10"/>
     </row>
     <row r="748" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A748" s="2"/>
-      <c r="B748" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C748" s="10" t="s">
-        <v>148</v>
-      </c>
+      <c r="A748" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B748" s="2"/>
+      <c r="C748" s="10"/>
     </row>
     <row r="749" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A749" s="2"/>
       <c r="B749" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C749" s="10" t="s">
-        <v>8</v>
+        <v>148</v>
       </c>
     </row>
     <row r="750" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A750" s="2"/>
       <c r="B750" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C750" s="11">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="C750" s="10" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="751" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A751" s="2"/>
       <c r="B751" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C751" s="10" t="s">
-        <v>163</v>
+        <v>3</v>
+      </c>
+      <c r="C751" s="11">
+        <v>1</v>
       </c>
     </row>
     <row r="752" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A752" s="2"/>
       <c r="B752" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="C752" s="5" t="s">
-        <v>175</v>
+        <v>11</v>
+      </c>
+      <c r="C752" s="10" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="753" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A753" s="2"/>
-      <c r="B753" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="C753" s="6" t="s">
-        <v>176</v>
+      <c r="B753" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C753" s="5" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="754" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A754" s="2"/>
-      <c r="B754" s="2"/>
-      <c r="C754" s="10"/>
+      <c r="B754" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C754" s="6" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="755" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A755" s="2" t="s">
-        <v>164</v>
-      </c>
+      <c r="A755" s="2"/>
       <c r="B755" s="2"/>
       <c r="C755" s="10"/>
     </row>
     <row r="756" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A756" s="2"/>
-      <c r="B756" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C756" s="10" t="s">
-        <v>148</v>
-      </c>
+      <c r="A756" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B756" s="2"/>
+      <c r="C756" s="10"/>
     </row>
     <row r="757" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A757" s="2"/>
       <c r="B757" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C757" s="10" t="s">
-        <v>8</v>
+        <v>148</v>
       </c>
     </row>
     <row r="758" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A758" s="2"/>
       <c r="B758" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C758" s="11">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="C758" s="10" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="759" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A759" s="2"/>
       <c r="B759" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C759" s="10" t="s">
-        <v>165</v>
+        <v>3</v>
+      </c>
+      <c r="C759" s="11">
+        <v>1</v>
       </c>
     </row>
     <row r="760" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A760" s="2"/>
       <c r="B760" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="C760" s="5" t="s">
-        <v>189</v>
+        <v>11</v>
+      </c>
+      <c r="C760" s="10" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="761" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A761" s="2"/>
-      <c r="B761" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="C761" s="6" t="s">
-        <v>190</v>
+      <c r="B761" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C761" s="5" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="762" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A762" s="2"/>
-      <c r="B762" s="2"/>
-      <c r="C762" s="10"/>
+      <c r="B762" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C762" s="6" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="763" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A763" s="2" t="s">
-        <v>191</v>
-      </c>
+      <c r="A763" s="2"/>
       <c r="B763" s="2"/>
       <c r="C763" s="10"/>
     </row>
     <row r="764" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A764" s="2"/>
-      <c r="B764" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C764" s="10" t="s">
-        <v>148</v>
-      </c>
+      <c r="A764" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B764" s="2"/>
+      <c r="C764" s="10"/>
     </row>
     <row r="765" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A765" s="2"/>
       <c r="B765" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C765" s="10" t="s">
-        <v>8</v>
+        <v>148</v>
       </c>
     </row>
     <row r="766" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A766" s="2"/>
       <c r="B766" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C766" s="11">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="C766" s="10" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="767" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A767" s="2"/>
       <c r="B767" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C767" s="10" t="s">
-        <v>192</v>
+        <v>3</v>
+      </c>
+      <c r="C767" s="11">
+        <v>1</v>
       </c>
     </row>
     <row r="768" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A768" s="2"/>
       <c r="B768" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="C768" s="5" t="s">
-        <v>189</v>
+        <v>11</v>
+      </c>
+      <c r="C768" s="10" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="769" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A769" s="2"/>
-      <c r="B769" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="C769" s="6" t="s">
-        <v>190</v>
+      <c r="B769" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C769" s="5" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="770" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A770" s="2"/>
-      <c r="B770" s="2"/>
-      <c r="C770" s="10"/>
+      <c r="B770" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C770" s="6" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="771" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A771" s="2" t="s">
-        <v>166</v>
-      </c>
+      <c r="A771" s="2"/>
       <c r="B771" s="2"/>
       <c r="C771" s="10"/>
     </row>
     <row r="772" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A772" s="2"/>
-      <c r="B772" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C772" s="10" t="s">
-        <v>148</v>
-      </c>
+      <c r="A772" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B772" s="2"/>
+      <c r="C772" s="10"/>
     </row>
     <row r="773" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A773" s="2"/>
       <c r="B773" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C773" s="10" t="s">
-        <v>8</v>
+        <v>148</v>
       </c>
     </row>
     <row r="774" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A774" s="2"/>
       <c r="B774" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C774" s="11">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="C774" s="10" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="775" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A775" s="2"/>
       <c r="B775" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C775" s="10" t="s">
-        <v>167</v>
+        <v>3</v>
+      </c>
+      <c r="C775" s="11">
+        <v>1</v>
       </c>
     </row>
     <row r="776" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A776" s="2"/>
       <c r="B776" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="C776" s="5" t="s">
-        <v>189</v>
+        <v>11</v>
+      </c>
+      <c r="C776" s="10" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="777" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A777" s="2"/>
-      <c r="B777" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="C777" s="6" t="s">
-        <v>190</v>
+      <c r="B777" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C777" s="5" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="778" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A778" s="2"/>
-      <c r="B778" s="2"/>
-      <c r="C778" s="10"/>
+      <c r="B778" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C778" s="6" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="779" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A779" s="2" t="s">
-        <v>168</v>
-      </c>
+      <c r="A779" s="2"/>
       <c r="B779" s="2"/>
       <c r="C779" s="10"/>
     </row>
     <row r="780" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A780" s="2"/>
-      <c r="B780" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C780" s="10" t="s">
-        <v>148</v>
-      </c>
+      <c r="A780" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B780" s="2"/>
+      <c r="C780" s="10"/>
     </row>
     <row r="781" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A781" s="2"/>
       <c r="B781" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C781" s="10" t="s">
-        <v>8</v>
+        <v>148</v>
       </c>
     </row>
     <row r="782" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A782" s="2"/>
       <c r="B782" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C782" s="11">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="C782" s="10" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="783" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A783" s="2"/>
       <c r="B783" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C783" s="10" t="s">
-        <v>169</v>
+        <v>3</v>
+      </c>
+      <c r="C783" s="11">
+        <v>1</v>
       </c>
     </row>
     <row r="784" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A784" s="2"/>
       <c r="B784" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="C784" s="5" t="s">
-        <v>189</v>
+        <v>11</v>
+      </c>
+      <c r="C784" s="10" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="785" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A785" s="2"/>
-      <c r="B785" s="9" t="s">
+      <c r="B785" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C785" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="786" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A786" s="2"/>
+      <c r="B786" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="C785" s="6" t="s">
+      <c r="C786" s="6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="787" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A787" s="2"/>
+      <c r="B787" s="2"/>
+      <c r="C787" s="10"/>
+    </row>
+    <row r="788" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A788" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B788" s="2"/>
+      <c r="C788" s="10"/>
+    </row>
+    <row r="789" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A789" s="2"/>
+      <c r="B789" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C789" s="10" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="790" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A790" s="2"/>
+      <c r="B790" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C790" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="791" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A791" s="2"/>
+      <c r="B791" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C791" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="792" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A792" s="2"/>
+      <c r="B792" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C792" s="10" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="793" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A793" s="2"/>
+      <c r="B793" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C793" s="5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="794" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A794" s="2"/>
+      <c r="B794" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C794" s="6" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="786" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="787" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="788" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="789" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="790" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="791" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="792" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="793" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="794" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="795" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="796" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="797" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="798" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="799" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="800" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="801" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="802" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="803" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="804" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="805" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="806" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="807" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="808" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="809" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="810" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="811" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="812" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="813" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="814" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="815" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="816" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="817" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="818" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="819" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="820" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="821" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="822" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="823" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="824" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="825" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="826" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="827" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="828" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="829" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="830" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="831" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="832" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="795" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A795" s="2"/>
+      <c r="B795" s="2"/>
+      <c r="C795" s="10"/>
+    </row>
+    <row r="796" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A796" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B796" s="2"/>
+      <c r="C796" s="10"/>
+    </row>
+    <row r="797" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A797" s="2"/>
+      <c r="B797" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C797" s="10" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="798" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A798" s="2"/>
+      <c r="B798" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C798" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="799" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A799" s="2"/>
+      <c r="B799" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C799" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="800" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A800" s="2"/>
+      <c r="B800" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C800" s="10" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="801" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A801" s="2"/>
+      <c r="B801" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C801" s="5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="802" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A802" s="2"/>
+      <c r="B802" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C802" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="803" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A803" s="2"/>
+      <c r="B803" s="2"/>
+      <c r="C803" s="10"/>
+    </row>
+    <row r="804" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A804" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B804" s="2"/>
+      <c r="C804" s="10"/>
+    </row>
+    <row r="805" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A805" s="2"/>
+      <c r="B805" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C805" s="10" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="806" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A806" s="2"/>
+      <c r="B806" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C806" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="807" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A807" s="2"/>
+      <c r="B807" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C807" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="808" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A808" s="2"/>
+      <c r="B808" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C808" s="10" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="809" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A809" s="2"/>
+      <c r="B809" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C809" s="5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="810" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A810" s="2"/>
+      <c r="B810" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C810" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="811" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A811" s="2"/>
+      <c r="B811" s="2"/>
+      <c r="C811" s="10"/>
+    </row>
+    <row r="812" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A812" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B812" s="2"/>
+      <c r="C812" s="10"/>
+    </row>
+    <row r="813" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A813" s="2"/>
+      <c r="B813" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C813" s="10" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="814" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A814" s="2"/>
+      <c r="B814" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C814" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="815" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A815" s="2"/>
+      <c r="B815" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C815" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="816" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A816" s="2"/>
+      <c r="B816" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C816" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="817" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A817" s="2"/>
+      <c r="B817" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C817" s="5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="818" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A818" s="2"/>
+      <c r="B818" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C818" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="819" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="820" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="821" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="822" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="823" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="824" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="825" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="826" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="827" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="828" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="829" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="830" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="831" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="832" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="833" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="834" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="835" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>